<commit_message>
Branch work, Speeedy 3/4, MEDY modified, 29/10
</commit_message>
<xml_diff>
--- a/TickerList.xlsx
+++ b/TickerList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kostayanev/easter/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kostayanev/NikyClean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E73EB64-4E58-B84D-8239-517AEB50CDB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77C6032-EFE6-A348-87A4-E620F81C72B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2880" yWindow="2000" windowWidth="27360" windowHeight="16440" xr2:uid="{9ADD1904-255D-1240-A5D2-DA49C36ED9E5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
   <si>
     <t>AAPL</t>
   </si>
@@ -631,7 +631,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7306280-7E31-7B4C-BC5F-D990252187FC}">
   <dimension ref="A1:B77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A75"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -672,336 +674,341 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>